<commit_message>
Fixed printing format on TC4-pins.xlsx
git-svn-id: http://tc4-shield.googlecode.com/svn@150 11eaef69-15cb-b3ff-657e-d52ce9b43f8f
</commit_message>
<xml_diff>
--- a/trunk/hardware/docs/TC4-pins.xlsx
+++ b/trunk/hardware/docs/TC4-pins.xlsx
@@ -823,10 +823,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F49"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -838,505 +841,519 @@
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:6">
-      <c r="A2" s="42" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="26">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>60</v>
+      <c r="F4" s="27" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="25" t="s">
-        <v>61</v>
-      </c>
+      <c r="D5" s="25"/>
       <c r="E5" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="D6" s="25"/>
       <c r="E6" s="26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>51</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>80</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="18" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="18" t="s">
-        <v>32</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="18"/>
       <c r="D9" s="25"/>
       <c r="E9" s="26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="25"/>
+      <c r="C10" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="28"/>
       <c r="E10" s="26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1">
       <c r="A11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="26">
-        <v>7</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>16</v>
+        <v>33</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="29">
+        <v>8</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1">
       <c r="A12" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="29">
-        <v>8</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1">
+        <v>34</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="31"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="31"/>
-    </row>
-    <row r="14" spans="1:6">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="46"/>
+      <c r="F13" s="47"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1">
+        <v>22</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="21"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="26">
         <v>1</v>
       </c>
-      <c r="F16" s="24" t="s">
-        <v>60</v>
+      <c r="F16" s="27" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>84</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D17" s="25"/>
       <c r="E17" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="A18" s="4"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="18" t="s">
-        <v>36</v>
-      </c>
+      <c r="C18" s="18"/>
       <c r="D18" s="25"/>
       <c r="E18" s="26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="4"/>
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="18"/>
+      <c r="C19" s="18" t="s">
+        <v>90</v>
+      </c>
       <c r="D19" s="25"/>
       <c r="E19" s="26">
-        <v>3</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>52</v>
+        <v>4</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26">
-        <v>4</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="18" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26">
-        <v>6</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>86</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1">
       <c r="A23" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1"/>
-      <c r="C23" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
+      <c r="C23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
+      <c r="A24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A25" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="26" spans="1:6">
+      <c r="A26" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
+    </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="35"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="36"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="37" t="s">
-        <v>55</v>
+      <c r="A28" s="36">
+        <v>1</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>70</v>
       </c>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="36">
-        <v>1</v>
+        <f>A28+1</f>
+        <v>2</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="36">
-        <f>A29+1</f>
-        <v>2</v>
+        <f t="shared" ref="A30:A41" si="0">A29+1</f>
+        <v>3</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>64</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="28" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="36">
-        <f t="shared" ref="A31:A42" si="0">A30+1</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28" t="s">
-        <v>73</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="28"/>
       <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="36">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="28"/>
+        <v>52</v>
+      </c>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28" t="s">
+        <v>56</v>
+      </c>
       <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="36">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28" t="s">
-        <v>56</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="28"/>
       <c r="F33" s="18"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="36">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28" t="s">
+        <v>57</v>
+      </c>
       <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="36">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C35" s="28"/>
       <c r="D35" s="28"/>
@@ -1348,10 +1365,10 @@
     <row r="36" spans="1:6">
       <c r="A36" s="36">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C36" s="28"/>
       <c r="D36" s="28"/>
@@ -1363,10 +1380,10 @@
     <row r="37" spans="1:6">
       <c r="A37" s="36">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
@@ -1378,31 +1395,33 @@
     <row r="38" spans="1:6">
       <c r="A38" s="36">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28" t="s">
-        <v>57</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="28"/>
       <c r="F38" s="18"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="36">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D39" s="28" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E39" s="28"/>
       <c r="F39" s="18"/>
@@ -1410,16 +1429,16 @@
     <row r="40" spans="1:6">
       <c r="A40" s="36">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E40" s="28"/>
       <c r="F40" s="18"/>
@@ -1427,96 +1446,82 @@
     <row r="41" spans="1:6">
       <c r="A41" s="36">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="E41" s="28"/>
       <c r="F41" s="18"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="36">
-        <f t="shared" si="0"/>
-        <v>14</v>
+      <c r="A42" s="38">
+        <v>15</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="E42" s="28"/>
+        <v>85</v>
+      </c>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28" t="s">
+        <v>74</v>
+      </c>
       <c r="F42" s="18"/>
     </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="38">
-        <v>15</v>
-      </c>
-      <c r="B43" s="28" t="s">
+    <row r="43" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A43" s="39">
+        <v>16</v>
+      </c>
+      <c r="B43" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="F43" s="18"/>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A44" s="39">
-        <v>16</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20" t="s">
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F44" s="21"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="17" t="s">
+      <c r="F43" s="21"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" thickBot="1"/>
-    <row r="48" spans="1:6">
-      <c r="A48" s="40" t="s">
+    <row r="46" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="47" spans="1:6">
+      <c r="A47" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="11"/>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A49" s="41" t="s">
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="11"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A48" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="7"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D13:F13"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="97" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;R&amp;D</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added note about SPI pins.
git-svn-id: http://tc4-shield.googlecode.com/svn@151 11eaef69-15cb-b3ff-657e-d52ce9b43f8f
</commit_message>
<xml_diff>
--- a/trunk/hardware/docs/TC4-pins.xlsx
+++ b/trunk/hardware/docs/TC4-pins.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="96">
   <si>
     <t>Arduino pin assignments</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Pin</t>
   </si>
   <si>
-    <t>Use</t>
-  </si>
-  <si>
     <t>D0</t>
   </si>
   <si>
@@ -60,12 +57,6 @@
     <t>D9</t>
   </si>
   <si>
-    <t>D10</t>
-  </si>
-  <si>
-    <t>D11</t>
-  </si>
-  <si>
     <t>D12</t>
   </si>
   <si>
@@ -292,6 +283,27 @@
   </si>
   <si>
     <t>ANLG2</t>
+  </si>
+  <si>
+    <t>TC4 Use</t>
+  </si>
+  <si>
+    <t>D10*</t>
+  </si>
+  <si>
+    <t>D11*</t>
+  </si>
+  <si>
+    <t>D12*</t>
+  </si>
+  <si>
+    <t>D13*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* These pins support SPI communication, which, although provided </t>
+  </si>
+  <si>
+    <t>by the underlying hardware, is not currently included in the Arduino language.</t>
   </si>
 </sst>
 </file>
@@ -438,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -529,6 +541,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,10 +839,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -848,7 +861,7 @@
       <c r="B1" s="43"/>
       <c r="C1" s="44"/>
       <c r="D1" s="45" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E1" s="46"/>
       <c r="F1" s="47"/>
@@ -866,45 +879,45 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E4" s="26">
         <v>1</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="25"/>
@@ -912,67 +925,67 @@
         <v>2</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="26">
         <v>3</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26">
         <v>4</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="26">
         <v>5</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="25"/>
@@ -980,50 +993,50 @@
         <v>6</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D10" s="28"/>
       <c r="E10" s="26">
         <v>7</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="29">
         <v>8</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1">
       <c r="A12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
@@ -1031,29 +1044,29 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" s="45" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E13" s="46"/>
       <c r="F13" s="47"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="20"/>
@@ -1061,54 +1074,54 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E16" s="26">
         <v>1</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="26">
         <v>2</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1120,64 +1133,64 @@
         <v>3</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="26">
         <v>4</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26">
         <v>5</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="26">
         <v>6</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="12"/>
@@ -1185,11 +1198,11 @@
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1">
       <c r="A23" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="14"/>
@@ -1197,231 +1210,225 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1">
       <c r="A24" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1"/>
-    <row r="26" spans="1:6">
-      <c r="A26" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="36"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="37" t="s">
+      <c r="A27" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="18"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="35"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="36">
-        <v>1</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="28" t="s">
+      <c r="A28" s="36"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="37" t="s">
         <v>52</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>70</v>
       </c>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="36">
-        <f>A28+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="36">
-        <f t="shared" ref="A30:A41" si="0">A29+1</f>
-        <v>3</v>
+        <f>A29+1</f>
+        <v>2</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
+        <v>35</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="E30" s="28" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="36">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" ref="A31:A42" si="0">A30+1</f>
+        <v>3</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="28"/>
+        <v>36</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28" t="s">
+        <v>70</v>
+      </c>
       <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="36">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28" t="s">
-        <v>56</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="28"/>
       <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="36">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="28"/>
+        <v>49</v>
+      </c>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28" t="s">
+        <v>53</v>
+      </c>
       <c r="F33" s="18"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="36">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28" t="s">
-        <v>57</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="28"/>
       <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="36">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C35" s="28"/>
       <c r="D35" s="28"/>
       <c r="E35" s="28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F35" s="18"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="36">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C36" s="28"/>
       <c r="D36" s="28"/>
       <c r="E36" s="28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="36">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
       <c r="E37" s="28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="36">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="F38" s="18"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="36">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D39" s="28" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E39" s="28"/>
       <c r="F39" s="18"/>
@@ -1429,16 +1436,16 @@
     <row r="40" spans="1:6">
       <c r="A40" s="36">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E40" s="28"/>
       <c r="F40" s="18"/>
@@ -1446,69 +1453,86 @@
     <row r="41" spans="1:6">
       <c r="A41" s="36">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E41" s="28"/>
       <c r="F41" s="18"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="38">
+      <c r="A42" s="36">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="38">
         <v>15</v>
       </c>
-      <c r="B42" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="F42" s="18"/>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A43" s="39">
+      <c r="B43" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A44" s="39">
         <v>16</v>
       </c>
-      <c r="B43" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F43" s="21"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="17" t="s">
+      <c r="B44" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" thickBot="1"/>
-    <row r="47" spans="1:6">
-      <c r="A47" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="11"/>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A48" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="7"/>
+      <c r="F44" s="21"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="48" spans="1:6">
+      <c r="A48" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A49" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>